<commit_message>
Fixed bug that was causing PayerCityStateZip to duplicate.
</commit_message>
<xml_diff>
--- a/data_source/invoice_data.xlsx
+++ b/data_source/invoice_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Name:</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Julie Smith</t>
+  </si>
+  <si>
+    <t>Austin, TX 78759</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,7 +482,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>